<commit_message>
Change Input file helper text to English
</commit_message>
<xml_diff>
--- a/Evaluate sorting algorithms.xlsx
+++ b/Evaluate sorting algorithms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://linuxvn-my.sharepoint.com/personal/ga59_linuxteamvietnam_edu_vn/Documents/UIT/Cấu trúc dữ liệu và giải thuật/evaluate-sorting-algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{6784F045-3861-49D4-AA08-3BE9A77498E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{121C8F6B-9766-4C77-8924-9576F3F4C0F1}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{6784F045-3861-49D4-AA08-3BE9A77498E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2169A150-916D-4F56-AC4E-C77DCD081EA0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{763B0E15-42E0-4774-993B-D559CEC4F9AD}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0\ \n\s"/>
     <numFmt numFmtId="165" formatCode="General\ \m\s"/>
@@ -264,7 +264,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{B4899899-8408-4107-BC83-13DD92AB2981}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -454,7 +456,7 @@
             <c:numRef>
               <c:f>'Execute time summary'!$C$6:$E$6</c:f>
               <c:numCache>
-                <c:formatCode>#,##0\ \n\s</c:formatCode>
+                <c:formatCode>#.##0\ \n\s</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1000000</c:v>
@@ -542,7 +544,7 @@
             <c:numRef>
               <c:f>'Execute time summary'!$C$7:$E$7</c:f>
               <c:numCache>
-                <c:formatCode>#,##0\ \n\s</c:formatCode>
+                <c:formatCode>#.##0\ \n\s</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -630,7 +632,7 @@
             <c:numRef>
               <c:f>'Execute time summary'!$C$8:$E$8</c:f>
               <c:numCache>
-                <c:formatCode>#,##0\ \n\s</c:formatCode>
+                <c:formatCode>#.##0\ \n\s</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -732,7 +734,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0\ \n\s" sourceLinked="1"/>
+        <c:numFmt formatCode="#.##0\ \n\s" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1071,7 +1073,7 @@
             <c:numRef>
               <c:f>'Execute time summary'!$F$6:$F$8</c:f>
               <c:numCache>
-                <c:formatCode>#,##0\ \n\s</c:formatCode>
+                <c:formatCode>#.##0\ \n\s</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>5666700</c:v>
@@ -1177,7 +1179,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0\ \n\s" sourceLinked="1"/>
+        <c:numFmt formatCode="#.##0\ \n\s" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1285,7 +1287,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Radix Sort</c:v>
+              <c:v>Interchange Sort</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1425,34 +1427,34 @@
                 <c:formatCode>General\ \m\s</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>277</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>352</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1562,34 +1564,34 @@
                 <c:formatCode>General\ \m\s</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>282</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>509</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>820</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>1223</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>1711</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>2266</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>2912</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>3861</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1699,34 +1701,34 @@
                 <c:formatCode>General\ \m\s</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>434</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>529</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>639</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1791,34 +1793,34 @@
                 <c:formatCode>General\ \m\s</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.66669999999999996</c:v>
+                  <c:v>5.6666999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66669999999999996</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>132.66669999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>232.33330000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3332999999999999</c:v>
+                  <c:v>366.66669999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6667000000000001</c:v>
+                  <c:v>535</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3332999999999999</c:v>
+                  <c:v>738.66669999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3332999999999999</c:v>
+                  <c:v>972.66669999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3332999999999999</c:v>
+                  <c:v>1239.3333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>1617.3333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3639,7 +3641,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" firstButton="1" fmlaLink="$A$1" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" firstButton="1" fmlaLink="$A$1" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3647,7 +3649,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4325,7 +4327,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4342,7 +4344,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4" t="str">
         <f>"Compare algorithms with n = " &amp;E2</f>
@@ -4361,7 +4363,7 @@
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="str">
         <f ca="1">INDIRECT("B"&amp;A1 + 5)</f>
-        <v>Radix Sort</v>
+        <v>Interchange Sort</v>
       </c>
       <c r="J3" s="10" t="str">
         <f t="array" aca="1" ref="J3:N13" ca="1">AlgorithmRadioButton</f>
@@ -4397,19 +4399,19 @@
       </c>
       <c r="K4" s="6">
         <f ca="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="M4" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="N4" s="6">
         <f ca="1"/>
-        <v>0.66669999999999996</v>
+        <v>5.6666999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4435,19 +4437,19 @@
       </c>
       <c r="K5" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L5" s="6">
         <f ca="1"/>
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="M5" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="N5" s="6">
         <f ca="1"/>
-        <v>0.66669999999999996</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -4479,19 +4481,19 @@
       </c>
       <c r="K6" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L6" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>282</v>
       </c>
       <c r="M6" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="N6" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>132.66669999999999</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -4523,19 +4525,19 @@
       </c>
       <c r="K7" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="L7" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>509</v>
       </c>
       <c r="M7" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="N7" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>232.33330000000001</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4567,19 +4569,19 @@
       </c>
       <c r="K8" s="6">
         <f ca="1"/>
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="L8" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>820</v>
       </c>
       <c r="M8" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="N8" s="6">
         <f ca="1"/>
-        <v>1.3332999999999999</v>
+        <v>366.66669999999999</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4589,19 +4591,19 @@
       </c>
       <c r="K9" s="6">
         <f ca="1"/>
-        <v>2</v>
+        <v>115</v>
       </c>
       <c r="L9" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>1223</v>
       </c>
       <c r="M9" s="6">
         <f ca="1"/>
-        <v>2</v>
+        <v>267</v>
       </c>
       <c r="N9" s="6">
         <f ca="1"/>
-        <v>1.6667000000000001</v>
+        <v>535</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -4611,19 +4613,19 @@
       </c>
       <c r="K10" s="6">
         <f ca="1"/>
-        <v>2</v>
+        <v>161</v>
       </c>
       <c r="L10" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>1711</v>
       </c>
       <c r="M10" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>344</v>
       </c>
       <c r="N10" s="6">
         <f ca="1"/>
-        <v>1.3332999999999999</v>
+        <v>738.66669999999999</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -4633,19 +4635,19 @@
       </c>
       <c r="K11" s="6">
         <f ca="1"/>
-        <v>3</v>
+        <v>218</v>
       </c>
       <c r="L11" s="6">
         <f ca="1"/>
-        <v>3</v>
+        <v>2266</v>
       </c>
       <c r="M11" s="6">
         <f ca="1"/>
-        <v>1</v>
+        <v>434</v>
       </c>
       <c r="N11" s="6">
         <f ca="1"/>
-        <v>2.3332999999999999</v>
+        <v>972.66669999999999</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -4655,19 +4657,19 @@
       </c>
       <c r="K12" s="6">
         <f ca="1"/>
-        <v>2</v>
+        <v>277</v>
       </c>
       <c r="L12" s="6">
         <f ca="1"/>
-        <v>3</v>
+        <v>2912</v>
       </c>
       <c r="M12" s="6">
         <f ca="1"/>
-        <v>2</v>
+        <v>529</v>
       </c>
       <c r="N12" s="6">
         <f ca="1"/>
-        <v>2.3332999999999999</v>
+        <v>1239.3333</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -4677,19 +4679,19 @@
       </c>
       <c r="K13" s="6">
         <f ca="1"/>
-        <v>3</v>
+        <v>352</v>
       </c>
       <c r="L13" s="6">
         <f ca="1"/>
-        <v>3</v>
+        <v>3861</v>
       </c>
       <c r="M13" s="6">
         <f ca="1"/>
-        <v>3</v>
+        <v>639</v>
       </c>
       <c r="N13" s="6">
         <f ca="1"/>
-        <v>3</v>
+        <v>1617.3333</v>
       </c>
     </row>
   </sheetData>
@@ -4777,7 +4779,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Nhập Input:" prompt="Chọn tập dữ liệu tương ứng với số lượng phần tử cần sắp xếp" xr:uid="{AB264513-C7C4-454B-BBBC-DF133826BF70}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Input file name:" prompt="Select the dataset corresponding to the number of elements to sort" xr:uid="{AB264513-C7C4-454B-BBBC-DF133826BF70}">
           <x14:formula1>
             <xm:f>'Interchange Sort'!$A$3:$A$13</xm:f>
           </x14:formula1>

</xml_diff>